<commit_message>
mark up Textvergleich und Validierung
mark up fuer die gleichen Stellen in TB_8 und MF_6-2 und mehrere Korrekturen im mark up
die Dateien wurden außerdem ersetzt mit jenen, die RH mit xml-IDs versehen hat.
Validierung der Dateien bis auf MF_6-2 - hier noch ein Problem
</commit_message>
<xml_diff>
--- a/docs/Uebersicht_Elemente_Baernreither-Edition_2023.xlsx
+++ b/docs/Uebersicht_Elemente_Baernreither-Edition_2023.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="144">
   <si>
     <t>Übersicht über die für Baernreither-Edition verwendeten Elemtente</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>subtypes? Zeitungsartikel, fremde, Baernreithers</t>
+  </si>
+  <si>
+    <t>"identical" gleicher Text in beiden Varianten; "missing" fehlt in der anderen Version</t>
   </si>
 </sst>
 </file>
@@ -872,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1572,88 +1575,92 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="5"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B65" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B66" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="12"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="12"/>
       <c r="B67" s="14"/>
       <c r="C67" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="13"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="12"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D68" s="13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B69" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="6"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D69" s="1"/>
-    </row>
-    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
       <c r="B70" s="9"/>
       <c r="C70" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A71" s="6"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
@@ -2189,6 +2196,12 @@
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
     </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
korrekturen markup TB8 und 7
Korrekturen markup
diary-entry ->diaryEntry
und Auszeichnung Tagebucheintraege
</commit_message>
<xml_diff>
--- a/docs/Uebersicht_Elemente_Baernreither-Edition_2023.xlsx
+++ b/docs/Uebersicht_Elemente_Baernreither-Edition_2023.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$4:$D$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$4:$D$67</definedName>
   </definedNames>
-  <calcPr calcId="150000" iterateDelta="1E-4"/>
+  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="144">
   <si>
     <t>Übersicht über die für Baernreither-Edition verwendeten Elemtente</t>
   </si>
@@ -451,6 +459,9 @@
   </si>
   <si>
     <t>"equal" gleicher Text in beiden Varianten; "notEqual" Text unterschiedlich; "missing" fehlt in der anderen Version</t>
+  </si>
+  <si>
+    <t>diaryEntry für Tagebucheintrag</t>
   </si>
 </sst>
 </file>
@@ -641,15 +652,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -919,7 +930,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -927,28 +938,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="135" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
-    <col min="2" max="2" width="34.375" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="80.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="80.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -956,13 +967,13 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -976,7 +987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>115</v>
       </c>
@@ -990,7 +1001,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1000,7 +1011,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -1010,7 +1021,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>119</v>
       </c>
@@ -1024,7 +1035,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="8"/>
       <c r="C9" s="5" t="s">
@@ -1034,7 +1045,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>123</v>
       </c>
@@ -1046,7 +1057,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>125</v>
       </c>
@@ -1060,7 +1071,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="8"/>
       <c r="C12" s="5" t="s">
@@ -1070,7 +1081,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1091,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -1090,7 +1101,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>52</v>
       </c>
@@ -1100,7 +1111,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
@@ -1114,7 +1125,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>31</v>
       </c>
@@ -1129,7 +1140,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="8"/>
       <c r="C18" s="5" t="s">
@@ -1140,7 +1151,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="8"/>
       <c r="C19" s="12" t="s">
@@ -1151,7 +1162,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>59</v>
       </c>
@@ -1165,1060 +1176,1068 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B23" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" s="21" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B25" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="20"/>
-    </row>
-    <row r="25" spans="1:5" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:5" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B27" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="20"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="C27" s="18"/>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B31" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C31" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D31" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="20"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="C34" s="5"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="C36" s="5"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" s="21" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B37" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="20"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="C37" s="18"/>
+      <c r="D37" s="20"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="5" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D39" s="13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+    <row r="40" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B40" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D40" s="20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="18" t="s">
+    <row r="41" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D41" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="42" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="C42" s="5"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="6" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E43" s="15"/>
-    </row>
-    <row r="44" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="5" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="C47" s="6"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="5" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="13"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B50" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="C50" s="6"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B51" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="C51" s="5"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B52" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B53" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="C53" s="5"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B54" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="55" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B55" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="56" spans="1:5" s="13" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="5"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="12"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D57" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="E56" s="17"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="E57" s="17"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B58" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="C60" s="5"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="C61" s="12"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="B62" s="8"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="B63" s="9"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B64" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="C64" s="5"/>
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B65" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+    <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B66" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="C66" s="6"/>
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B67" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="1"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="5"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E68" s="1"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
     </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:D66"/>
+  <autoFilter ref="A4:D67"/>
   <sortState ref="A5:E72">
     <sortCondition ref="A5"/>
   </sortState>

</xml_diff>